<commit_message>
endringer for scenarioer og fuelcost2
</commit_message>
<xml_diff>
--- a/run_model/SetData-sheets.xlsx
+++ b/run_model/SetData-sheets.xlsx
@@ -13,9 +13,10 @@
     <sheet name="Time periods" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="Time periods 1" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="Time periods 2" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Fuel types" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="Installations" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="Scenarios" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="TP2 scrap" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Fuel types" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Installations" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="Scenarios" sheetId="10" state="visible" r:id="rId10"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -508,6 +509,57 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Scenarios</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
@@ -9824,6 +9876,57 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>TP2 scrap</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9889,7 +9992,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -10003,80 +10106,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Scenarios</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Lagt til CCS og oppdatert scengen
</commit_message>
<xml_diff>
--- a/run_model/SetData-sheets.xlsx
+++ b/run_model/SetData-sheets.xlsx
@@ -434,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A12"/>
+  <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -504,6 +504,16 @@
         <v>11</v>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -515,7 +525,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -533,6 +543,136 @@
     <row r="2">
       <c r="A2" t="n">
         <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -602,7 +742,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1063"/>
+  <dimension ref="A1:A859"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4905,1026 +5045,6 @@
     <row r="859">
       <c r="A859" t="n">
         <v>858</v>
-      </c>
-    </row>
-    <row r="860">
-      <c r="A860" t="n">
-        <v>859</v>
-      </c>
-    </row>
-    <row r="861">
-      <c r="A861" t="n">
-        <v>860</v>
-      </c>
-    </row>
-    <row r="862">
-      <c r="A862" t="n">
-        <v>861</v>
-      </c>
-    </row>
-    <row r="863">
-      <c r="A863" t="n">
-        <v>862</v>
-      </c>
-    </row>
-    <row r="864">
-      <c r="A864" t="n">
-        <v>863</v>
-      </c>
-    </row>
-    <row r="865">
-      <c r="A865" t="n">
-        <v>864</v>
-      </c>
-    </row>
-    <row r="866">
-      <c r="A866" t="n">
-        <v>865</v>
-      </c>
-    </row>
-    <row r="867">
-      <c r="A867" t="n">
-        <v>866</v>
-      </c>
-    </row>
-    <row r="868">
-      <c r="A868" t="n">
-        <v>867</v>
-      </c>
-    </row>
-    <row r="869">
-      <c r="A869" t="n">
-        <v>868</v>
-      </c>
-    </row>
-    <row r="870">
-      <c r="A870" t="n">
-        <v>869</v>
-      </c>
-    </row>
-    <row r="871">
-      <c r="A871" t="n">
-        <v>870</v>
-      </c>
-    </row>
-    <row r="872">
-      <c r="A872" t="n">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="873">
-      <c r="A873" t="n">
-        <v>872</v>
-      </c>
-    </row>
-    <row r="874">
-      <c r="A874" t="n">
-        <v>873</v>
-      </c>
-    </row>
-    <row r="875">
-      <c r="A875" t="n">
-        <v>874</v>
-      </c>
-    </row>
-    <row r="876">
-      <c r="A876" t="n">
-        <v>875</v>
-      </c>
-    </row>
-    <row r="877">
-      <c r="A877" t="n">
-        <v>876</v>
-      </c>
-    </row>
-    <row r="878">
-      <c r="A878" t="n">
-        <v>877</v>
-      </c>
-    </row>
-    <row r="879">
-      <c r="A879" t="n">
-        <v>878</v>
-      </c>
-    </row>
-    <row r="880">
-      <c r="A880" t="n">
-        <v>879</v>
-      </c>
-    </row>
-    <row r="881">
-      <c r="A881" t="n">
-        <v>880</v>
-      </c>
-    </row>
-    <row r="882">
-      <c r="A882" t="n">
-        <v>881</v>
-      </c>
-    </row>
-    <row r="883">
-      <c r="A883" t="n">
-        <v>882</v>
-      </c>
-    </row>
-    <row r="884">
-      <c r="A884" t="n">
-        <v>883</v>
-      </c>
-    </row>
-    <row r="885">
-      <c r="A885" t="n">
-        <v>884</v>
-      </c>
-    </row>
-    <row r="886">
-      <c r="A886" t="n">
-        <v>885</v>
-      </c>
-    </row>
-    <row r="887">
-      <c r="A887" t="n">
-        <v>886</v>
-      </c>
-    </row>
-    <row r="888">
-      <c r="A888" t="n">
-        <v>887</v>
-      </c>
-    </row>
-    <row r="889">
-      <c r="A889" t="n">
-        <v>888</v>
-      </c>
-    </row>
-    <row r="890">
-      <c r="A890" t="n">
-        <v>889</v>
-      </c>
-    </row>
-    <row r="891">
-      <c r="A891" t="n">
-        <v>890</v>
-      </c>
-    </row>
-    <row r="892">
-      <c r="A892" t="n">
-        <v>891</v>
-      </c>
-    </row>
-    <row r="893">
-      <c r="A893" t="n">
-        <v>892</v>
-      </c>
-    </row>
-    <row r="894">
-      <c r="A894" t="n">
-        <v>893</v>
-      </c>
-    </row>
-    <row r="895">
-      <c r="A895" t="n">
-        <v>894</v>
-      </c>
-    </row>
-    <row r="896">
-      <c r="A896" t="n">
-        <v>895</v>
-      </c>
-    </row>
-    <row r="897">
-      <c r="A897" t="n">
-        <v>896</v>
-      </c>
-    </row>
-    <row r="898">
-      <c r="A898" t="n">
-        <v>897</v>
-      </c>
-    </row>
-    <row r="899">
-      <c r="A899" t="n">
-        <v>898</v>
-      </c>
-    </row>
-    <row r="900">
-      <c r="A900" t="n">
-        <v>899</v>
-      </c>
-    </row>
-    <row r="901">
-      <c r="A901" t="n">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="902">
-      <c r="A902" t="n">
-        <v>901</v>
-      </c>
-    </row>
-    <row r="903">
-      <c r="A903" t="n">
-        <v>902</v>
-      </c>
-    </row>
-    <row r="904">
-      <c r="A904" t="n">
-        <v>903</v>
-      </c>
-    </row>
-    <row r="905">
-      <c r="A905" t="n">
-        <v>904</v>
-      </c>
-    </row>
-    <row r="906">
-      <c r="A906" t="n">
-        <v>905</v>
-      </c>
-    </row>
-    <row r="907">
-      <c r="A907" t="n">
-        <v>906</v>
-      </c>
-    </row>
-    <row r="908">
-      <c r="A908" t="n">
-        <v>907</v>
-      </c>
-    </row>
-    <row r="909">
-      <c r="A909" t="n">
-        <v>908</v>
-      </c>
-    </row>
-    <row r="910">
-      <c r="A910" t="n">
-        <v>909</v>
-      </c>
-    </row>
-    <row r="911">
-      <c r="A911" t="n">
-        <v>910</v>
-      </c>
-    </row>
-    <row r="912">
-      <c r="A912" t="n">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="913">
-      <c r="A913" t="n">
-        <v>912</v>
-      </c>
-    </row>
-    <row r="914">
-      <c r="A914" t="n">
-        <v>913</v>
-      </c>
-    </row>
-    <row r="915">
-      <c r="A915" t="n">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="916">
-      <c r="A916" t="n">
-        <v>915</v>
-      </c>
-    </row>
-    <row r="917">
-      <c r="A917" t="n">
-        <v>916</v>
-      </c>
-    </row>
-    <row r="918">
-      <c r="A918" t="n">
-        <v>917</v>
-      </c>
-    </row>
-    <row r="919">
-      <c r="A919" t="n">
-        <v>918</v>
-      </c>
-    </row>
-    <row r="920">
-      <c r="A920" t="n">
-        <v>919</v>
-      </c>
-    </row>
-    <row r="921">
-      <c r="A921" t="n">
-        <v>920</v>
-      </c>
-    </row>
-    <row r="922">
-      <c r="A922" t="n">
-        <v>921</v>
-      </c>
-    </row>
-    <row r="923">
-      <c r="A923" t="n">
-        <v>922</v>
-      </c>
-    </row>
-    <row r="924">
-      <c r="A924" t="n">
-        <v>923</v>
-      </c>
-    </row>
-    <row r="925">
-      <c r="A925" t="n">
-        <v>924</v>
-      </c>
-    </row>
-    <row r="926">
-      <c r="A926" t="n">
-        <v>925</v>
-      </c>
-    </row>
-    <row r="927">
-      <c r="A927" t="n">
-        <v>926</v>
-      </c>
-    </row>
-    <row r="928">
-      <c r="A928" t="n">
-        <v>927</v>
-      </c>
-    </row>
-    <row r="929">
-      <c r="A929" t="n">
-        <v>928</v>
-      </c>
-    </row>
-    <row r="930">
-      <c r="A930" t="n">
-        <v>929</v>
-      </c>
-    </row>
-    <row r="931">
-      <c r="A931" t="n">
-        <v>930</v>
-      </c>
-    </row>
-    <row r="932">
-      <c r="A932" t="n">
-        <v>931</v>
-      </c>
-    </row>
-    <row r="933">
-      <c r="A933" t="n">
-        <v>932</v>
-      </c>
-    </row>
-    <row r="934">
-      <c r="A934" t="n">
-        <v>933</v>
-      </c>
-    </row>
-    <row r="935">
-      <c r="A935" t="n">
-        <v>934</v>
-      </c>
-    </row>
-    <row r="936">
-      <c r="A936" t="n">
-        <v>935</v>
-      </c>
-    </row>
-    <row r="937">
-      <c r="A937" t="n">
-        <v>936</v>
-      </c>
-    </row>
-    <row r="938">
-      <c r="A938" t="n">
-        <v>937</v>
-      </c>
-    </row>
-    <row r="939">
-      <c r="A939" t="n">
-        <v>938</v>
-      </c>
-    </row>
-    <row r="940">
-      <c r="A940" t="n">
-        <v>939</v>
-      </c>
-    </row>
-    <row r="941">
-      <c r="A941" t="n">
-        <v>940</v>
-      </c>
-    </row>
-    <row r="942">
-      <c r="A942" t="n">
-        <v>941</v>
-      </c>
-    </row>
-    <row r="943">
-      <c r="A943" t="n">
-        <v>942</v>
-      </c>
-    </row>
-    <row r="944">
-      <c r="A944" t="n">
-        <v>943</v>
-      </c>
-    </row>
-    <row r="945">
-      <c r="A945" t="n">
-        <v>944</v>
-      </c>
-    </row>
-    <row r="946">
-      <c r="A946" t="n">
-        <v>945</v>
-      </c>
-    </row>
-    <row r="947">
-      <c r="A947" t="n">
-        <v>946</v>
-      </c>
-    </row>
-    <row r="948">
-      <c r="A948" t="n">
-        <v>947</v>
-      </c>
-    </row>
-    <row r="949">
-      <c r="A949" t="n">
-        <v>948</v>
-      </c>
-    </row>
-    <row r="950">
-      <c r="A950" t="n">
-        <v>949</v>
-      </c>
-    </row>
-    <row r="951">
-      <c r="A951" t="n">
-        <v>950</v>
-      </c>
-    </row>
-    <row r="952">
-      <c r="A952" t="n">
-        <v>951</v>
-      </c>
-    </row>
-    <row r="953">
-      <c r="A953" t="n">
-        <v>952</v>
-      </c>
-    </row>
-    <row r="954">
-      <c r="A954" t="n">
-        <v>953</v>
-      </c>
-    </row>
-    <row r="955">
-      <c r="A955" t="n">
-        <v>954</v>
-      </c>
-    </row>
-    <row r="956">
-      <c r="A956" t="n">
-        <v>955</v>
-      </c>
-    </row>
-    <row r="957">
-      <c r="A957" t="n">
-        <v>956</v>
-      </c>
-    </row>
-    <row r="958">
-      <c r="A958" t="n">
-        <v>957</v>
-      </c>
-    </row>
-    <row r="959">
-      <c r="A959" t="n">
-        <v>958</v>
-      </c>
-    </row>
-    <row r="960">
-      <c r="A960" t="n">
-        <v>959</v>
-      </c>
-    </row>
-    <row r="961">
-      <c r="A961" t="n">
-        <v>960</v>
-      </c>
-    </row>
-    <row r="962">
-      <c r="A962" t="n">
-        <v>961</v>
-      </c>
-    </row>
-    <row r="963">
-      <c r="A963" t="n">
-        <v>962</v>
-      </c>
-    </row>
-    <row r="964">
-      <c r="A964" t="n">
-        <v>963</v>
-      </c>
-    </row>
-    <row r="965">
-      <c r="A965" t="n">
-        <v>964</v>
-      </c>
-    </row>
-    <row r="966">
-      <c r="A966" t="n">
-        <v>965</v>
-      </c>
-    </row>
-    <row r="967">
-      <c r="A967" t="n">
-        <v>966</v>
-      </c>
-    </row>
-    <row r="968">
-      <c r="A968" t="n">
-        <v>967</v>
-      </c>
-    </row>
-    <row r="969">
-      <c r="A969" t="n">
-        <v>968</v>
-      </c>
-    </row>
-    <row r="970">
-      <c r="A970" t="n">
-        <v>969</v>
-      </c>
-    </row>
-    <row r="971">
-      <c r="A971" t="n">
-        <v>970</v>
-      </c>
-    </row>
-    <row r="972">
-      <c r="A972" t="n">
-        <v>971</v>
-      </c>
-    </row>
-    <row r="973">
-      <c r="A973" t="n">
-        <v>972</v>
-      </c>
-    </row>
-    <row r="974">
-      <c r="A974" t="n">
-        <v>973</v>
-      </c>
-    </row>
-    <row r="975">
-      <c r="A975" t="n">
-        <v>974</v>
-      </c>
-    </row>
-    <row r="976">
-      <c r="A976" t="n">
-        <v>975</v>
-      </c>
-    </row>
-    <row r="977">
-      <c r="A977" t="n">
-        <v>976</v>
-      </c>
-    </row>
-    <row r="978">
-      <c r="A978" t="n">
-        <v>977</v>
-      </c>
-    </row>
-    <row r="979">
-      <c r="A979" t="n">
-        <v>978</v>
-      </c>
-    </row>
-    <row r="980">
-      <c r="A980" t="n">
-        <v>979</v>
-      </c>
-    </row>
-    <row r="981">
-      <c r="A981" t="n">
-        <v>980</v>
-      </c>
-    </row>
-    <row r="982">
-      <c r="A982" t="n">
-        <v>981</v>
-      </c>
-    </row>
-    <row r="983">
-      <c r="A983" t="n">
-        <v>982</v>
-      </c>
-    </row>
-    <row r="984">
-      <c r="A984" t="n">
-        <v>983</v>
-      </c>
-    </row>
-    <row r="985">
-      <c r="A985" t="n">
-        <v>984</v>
-      </c>
-    </row>
-    <row r="986">
-      <c r="A986" t="n">
-        <v>985</v>
-      </c>
-    </row>
-    <row r="987">
-      <c r="A987" t="n">
-        <v>986</v>
-      </c>
-    </row>
-    <row r="988">
-      <c r="A988" t="n">
-        <v>987</v>
-      </c>
-    </row>
-    <row r="989">
-      <c r="A989" t="n">
-        <v>988</v>
-      </c>
-    </row>
-    <row r="990">
-      <c r="A990" t="n">
-        <v>989</v>
-      </c>
-    </row>
-    <row r="991">
-      <c r="A991" t="n">
-        <v>990</v>
-      </c>
-    </row>
-    <row r="992">
-      <c r="A992" t="n">
-        <v>991</v>
-      </c>
-    </row>
-    <row r="993">
-      <c r="A993" t="n">
-        <v>992</v>
-      </c>
-    </row>
-    <row r="994">
-      <c r="A994" t="n">
-        <v>993</v>
-      </c>
-    </row>
-    <row r="995">
-      <c r="A995" t="n">
-        <v>994</v>
-      </c>
-    </row>
-    <row r="996">
-      <c r="A996" t="n">
-        <v>995</v>
-      </c>
-    </row>
-    <row r="997">
-      <c r="A997" t="n">
-        <v>996</v>
-      </c>
-    </row>
-    <row r="998">
-      <c r="A998" t="n">
-        <v>997</v>
-      </c>
-    </row>
-    <row r="999">
-      <c r="A999" t="n">
-        <v>998</v>
-      </c>
-    </row>
-    <row r="1000">
-      <c r="A1000" t="n">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="1001">
-      <c r="A1001" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="1002">
-      <c r="A1002" t="n">
-        <v>1001</v>
-      </c>
-    </row>
-    <row r="1003">
-      <c r="A1003" t="n">
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="1004">
-      <c r="A1004" t="n">
-        <v>1003</v>
-      </c>
-    </row>
-    <row r="1005">
-      <c r="A1005" t="n">
-        <v>1004</v>
-      </c>
-    </row>
-    <row r="1006">
-      <c r="A1006" t="n">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="1007">
-      <c r="A1007" t="n">
-        <v>1006</v>
-      </c>
-    </row>
-    <row r="1008">
-      <c r="A1008" t="n">
-        <v>1007</v>
-      </c>
-    </row>
-    <row r="1009">
-      <c r="A1009" t="n">
-        <v>1008</v>
-      </c>
-    </row>
-    <row r="1010">
-      <c r="A1010" t="n">
-        <v>1009</v>
-      </c>
-    </row>
-    <row r="1011">
-      <c r="A1011" t="n">
-        <v>1010</v>
-      </c>
-    </row>
-    <row r="1012">
-      <c r="A1012" t="n">
-        <v>1011</v>
-      </c>
-    </row>
-    <row r="1013">
-      <c r="A1013" t="n">
-        <v>1012</v>
-      </c>
-    </row>
-    <row r="1014">
-      <c r="A1014" t="n">
-        <v>1013</v>
-      </c>
-    </row>
-    <row r="1015">
-      <c r="A1015" t="n">
-        <v>1014</v>
-      </c>
-    </row>
-    <row r="1016">
-      <c r="A1016" t="n">
-        <v>1015</v>
-      </c>
-    </row>
-    <row r="1017">
-      <c r="A1017" t="n">
-        <v>1016</v>
-      </c>
-    </row>
-    <row r="1018">
-      <c r="A1018" t="n">
-        <v>1017</v>
-      </c>
-    </row>
-    <row r="1019">
-      <c r="A1019" t="n">
-        <v>1018</v>
-      </c>
-    </row>
-    <row r="1020">
-      <c r="A1020" t="n">
-        <v>1019</v>
-      </c>
-    </row>
-    <row r="1021">
-      <c r="A1021" t="n">
-        <v>1020</v>
-      </c>
-    </row>
-    <row r="1022">
-      <c r="A1022" t="n">
-        <v>1021</v>
-      </c>
-    </row>
-    <row r="1023">
-      <c r="A1023" t="n">
-        <v>1022</v>
-      </c>
-    </row>
-    <row r="1024">
-      <c r="A1024" t="n">
-        <v>1023</v>
-      </c>
-    </row>
-    <row r="1025">
-      <c r="A1025" t="n">
-        <v>1024</v>
-      </c>
-    </row>
-    <row r="1026">
-      <c r="A1026" t="n">
-        <v>1025</v>
-      </c>
-    </row>
-    <row r="1027">
-      <c r="A1027" t="n">
-        <v>1026</v>
-      </c>
-    </row>
-    <row r="1028">
-      <c r="A1028" t="n">
-        <v>1027</v>
-      </c>
-    </row>
-    <row r="1029">
-      <c r="A1029" t="n">
-        <v>1028</v>
-      </c>
-    </row>
-    <row r="1030">
-      <c r="A1030" t="n">
-        <v>1029</v>
-      </c>
-    </row>
-    <row r="1031">
-      <c r="A1031" t="n">
-        <v>1030</v>
-      </c>
-    </row>
-    <row r="1032">
-      <c r="A1032" t="n">
-        <v>1031</v>
-      </c>
-    </row>
-    <row r="1033">
-      <c r="A1033" t="n">
-        <v>1032</v>
-      </c>
-    </row>
-    <row r="1034">
-      <c r="A1034" t="n">
-        <v>1033</v>
-      </c>
-    </row>
-    <row r="1035">
-      <c r="A1035" t="n">
-        <v>1034</v>
-      </c>
-    </row>
-    <row r="1036">
-      <c r="A1036" t="n">
-        <v>1035</v>
-      </c>
-    </row>
-    <row r="1037">
-      <c r="A1037" t="n">
-        <v>1036</v>
-      </c>
-    </row>
-    <row r="1038">
-      <c r="A1038" t="n">
-        <v>1037</v>
-      </c>
-    </row>
-    <row r="1039">
-      <c r="A1039" t="n">
-        <v>1038</v>
-      </c>
-    </row>
-    <row r="1040">
-      <c r="A1040" t="n">
-        <v>1039</v>
-      </c>
-    </row>
-    <row r="1041">
-      <c r="A1041" t="n">
-        <v>1040</v>
-      </c>
-    </row>
-    <row r="1042">
-      <c r="A1042" t="n">
-        <v>1041</v>
-      </c>
-    </row>
-    <row r="1043">
-      <c r="A1043" t="n">
-        <v>1042</v>
-      </c>
-    </row>
-    <row r="1044">
-      <c r="A1044" t="n">
-        <v>1043</v>
-      </c>
-    </row>
-    <row r="1045">
-      <c r="A1045" t="n">
-        <v>1044</v>
-      </c>
-    </row>
-    <row r="1046">
-      <c r="A1046" t="n">
-        <v>1045</v>
-      </c>
-    </row>
-    <row r="1047">
-      <c r="A1047" t="n">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="1048">
-      <c r="A1048" t="n">
-        <v>1047</v>
-      </c>
-    </row>
-    <row r="1049">
-      <c r="A1049" t="n">
-        <v>1048</v>
-      </c>
-    </row>
-    <row r="1050">
-      <c r="A1050" t="n">
-        <v>1049</v>
-      </c>
-    </row>
-    <row r="1051">
-      <c r="A1051" t="n">
-        <v>1050</v>
-      </c>
-    </row>
-    <row r="1052">
-      <c r="A1052" t="n">
-        <v>1051</v>
-      </c>
-    </row>
-    <row r="1053">
-      <c r="A1053" t="n">
-        <v>1052</v>
-      </c>
-    </row>
-    <row r="1054">
-      <c r="A1054" t="n">
-        <v>1053</v>
-      </c>
-    </row>
-    <row r="1055">
-      <c r="A1055" t="n">
-        <v>1054</v>
-      </c>
-    </row>
-    <row r="1056">
-      <c r="A1056" t="n">
-        <v>1055</v>
-      </c>
-    </row>
-    <row r="1057">
-      <c r="A1057" t="n">
-        <v>1056</v>
-      </c>
-    </row>
-    <row r="1058">
-      <c r="A1058" t="n">
-        <v>1057</v>
-      </c>
-    </row>
-    <row r="1059">
-      <c r="A1059" t="n">
-        <v>1058</v>
-      </c>
-    </row>
-    <row r="1060">
-      <c r="A1060" t="n">
-        <v>1059</v>
-      </c>
-    </row>
-    <row r="1061">
-      <c r="A1061" t="n">
-        <v>1060</v>
-      </c>
-    </row>
-    <row r="1062">
-      <c r="A1062" t="n">
-        <v>1061</v>
-      </c>
-    </row>
-    <row r="1063">
-      <c r="A1063" t="n">
-        <v>1062</v>
       </c>
     </row>
   </sheetData>
@@ -6183,7 +5303,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A17"/>
+  <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6253,31 +5373,6 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>16</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Ruter og acc model
</commit_message>
<xml_diff>
--- a/run_model/SetData-sheets.xlsx
+++ b/run_model/SetData-sheets.xlsx
@@ -500,7 +500,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A28"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -518,136 +518,6 @@
     <row r="2">
       <c r="A2" t="n">
         <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="n">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="n">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="n">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="n">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="n">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="n">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="n">
-        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -717,7 +587,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A40"/>
+  <dimension ref="A1:A27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -860,71 +730,6 @@
     <row r="27">
       <c r="A27" t="n">
         <v>26</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="n">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="n">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="n">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="n">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="n">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="n">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="n">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="n">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="n">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="n">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="n">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="n">
-        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1183,7 +988,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A12"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1228,31 +1033,6 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>11</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
VSS og skrive ut kostnader
</commit_message>
<xml_diff>
--- a/run_model/SetData-sheets.xlsx
+++ b/run_model/SetData-sheets.xlsx
@@ -500,7 +500,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -518,6 +518,136 @@
     <row r="2">
       <c r="A2" t="n">
         <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>